<commit_message>
update test file for computed columns
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="149">
   <si>
     <t>text</t>
   </si>
@@ -452,6 +452,24 @@
   </si>
   <si>
     <t>org</t>
+  </si>
+  <si>
+    <t>xcomputedint</t>
+  </si>
+  <si>
+    <t>expression</t>
+  </si>
+  <si>
+    <t>xcomputedxref</t>
+  </si>
+  <si>
+    <t>abstract</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>{Chromosome: xstring, Position: xint}</t>
   </si>
 </sst>
 </file>
@@ -500,9 +518,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -515,13 +534,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -824,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AM39" sqref="AM39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5009,20 +5029,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5032,8 +5052,11 @@
       <c r="C1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -5044,7 +5067,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -5054,6 +5077,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5064,24 +5088,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:P45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD43"/>
+      <selection activeCell="P45" sqref="P45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5127,8 +5152,11 @@
       <c r="O1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5148,7 +5176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -5171,7 +5199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -5191,7 +5219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -5211,7 +5239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -5231,7 +5259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -5251,7 +5279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -5271,7 +5299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -5291,7 +5319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -5308,7 +5336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -5325,7 +5353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -5345,7 +5373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -5365,7 +5393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -5382,7 +5410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -5402,7 +5430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -5748,7 +5776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:16">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -5768,7 +5796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:16">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -5785,7 +5813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:16">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -5802,7 +5830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:16">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -5819,7 +5847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:16">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -5842,7 +5870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:16">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -5862,7 +5890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:16">
       <c r="A39" t="s">
         <v>95</v>
       </c>
@@ -5882,7 +5910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:16">
       <c r="A40" t="s">
         <v>96</v>
       </c>
@@ -5902,7 +5930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:16">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -5922,7 +5950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:16">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -5942,7 +5970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:16">
       <c r="A43" t="s">
         <v>136</v>
       </c>
@@ -5963,6 +5991,55 @@
       </c>
       <c r="O43" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" t="s">
+        <v>145</v>
+      </c>
+      <c r="B44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" t="s">
+        <v>78</v>
+      </c>
+      <c r="D44" t="s">
+        <v>147</v>
+      </c>
+      <c r="E44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
+      <c r="L44" t="b">
+        <v>1</v>
+      </c>
+      <c r="P44" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" t="s">
+        <v>143</v>
+      </c>
+      <c r="B45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45" t="b">
+        <v>1</v>
+      </c>
+      <c r="L45" t="b">
+        <v>1</v>
+      </c>
+      <c r="P45" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
One type of Repository end capabilities
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16440" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="143">
   <si>
     <t>text</t>
   </si>
@@ -452,21 +452,6 @@
   </si>
   <si>
     <t>org</t>
-  </si>
-  <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>sf</t>
   </si>
 </sst>
 </file>
@@ -837,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP39"/>
+  <dimension ref="A1:AN39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AP11" sqref="AP11"/>
+    <sheetView topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AO1" sqref="AO1:AP6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -868,7 +853,7 @@
     <col min="38" max="38" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42">
+    <row r="1" spans="1:40">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -989,14 +974,8 @@
       <c r="AN1" t="s">
         <v>136</v>
       </c>
-      <c r="AO1" t="s">
-        <v>138</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="2" spans="1:42">
+    </row>
+    <row r="2" spans="1:40">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1117,14 +1096,8 @@
       <c r="AN2" t="s">
         <v>2</v>
       </c>
-      <c r="AO2" t="s">
-        <v>144</v>
-      </c>
-      <c r="AP2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:42">
+    </row>
+    <row r="3" spans="1:40">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1245,14 +1218,8 @@
       <c r="AN3" t="s">
         <v>3</v>
       </c>
-      <c r="AO3" t="s">
-        <v>145</v>
-      </c>
-      <c r="AP3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:42">
+    </row>
+    <row r="4" spans="1:40">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1322,14 +1289,8 @@
       <c r="AN4" t="s">
         <v>4</v>
       </c>
-      <c r="AO4" t="s">
-        <v>145</v>
-      </c>
-      <c r="AP4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:42">
+    </row>
+    <row r="5" spans="1:40">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1450,14 +1411,8 @@
       <c r="AN5" t="s">
         <v>53</v>
       </c>
-      <c r="AO5" t="s">
-        <v>146</v>
-      </c>
-      <c r="AP5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:42">
+    </row>
+    <row r="6" spans="1:40">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1578,11 +1533,8 @@
       <c r="AN6" t="s">
         <v>54</v>
       </c>
-      <c r="AO6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="7" spans="1:42">
+    </row>
+    <row r="7" spans="1:40">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1650,7 +1602,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:42">
+    <row r="8" spans="1:40">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1769,7 +1721,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:42">
+    <row r="9" spans="1:40">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1888,7 +1840,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:42">
+    <row r="10" spans="1:40">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1956,7 +1908,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:42">
+    <row r="11" spans="1:40">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2075,7 +2027,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:42">
+    <row r="12" spans="1:40">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2194,7 +2146,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:42">
+    <row r="13" spans="1:40">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2262,7 +2214,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:42">
+    <row r="14" spans="1:40">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2381,7 +2333,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:42">
+    <row r="15" spans="1:40">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2500,7 +2452,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:42">
+    <row r="16" spans="1:40">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5112,10 +5064,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O45"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6013,40 +5965,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:15">
-      <c r="A44" t="s">
-        <v>138</v>
-      </c>
-      <c r="B44" t="s">
-        <v>57</v>
-      </c>
-      <c r="C44" t="s">
-        <v>66</v>
-      </c>
-      <c r="E44" t="b">
-        <v>0</v>
-      </c>
-      <c r="F44" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15">
-      <c r="A45" t="s">
-        <v>143</v>
-      </c>
-      <c r="B45" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" t="s">
-        <v>67</v>
-      </c>
-      <c r="E45" t="b">
-        <v>0</v>
-      </c>
-      <c r="F45" t="b">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Refactor indexed repos. Reindexing
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="146">
   <si>
     <t>text</t>
   </si>
@@ -452,6 +452,15 @@
   </si>
   <si>
     <t>org</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>dsd</t>
+  </si>
+  <si>
+    <t>dssss</t>
   </si>
 </sst>
 </file>
@@ -822,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN39"/>
+  <dimension ref="A1:AO39"/>
   <sheetViews>
     <sheetView topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AO1" sqref="AO1:AP6"/>
+      <selection activeCell="AO3" sqref="AO3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -853,7 +862,7 @@
     <col min="38" max="38" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:41">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -974,8 +983,11 @@
       <c r="AN1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="2" spans="1:40">
+      <c r="AO1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1096,8 +1108,11 @@
       <c r="AN2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:40">
+      <c r="AO2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1218,8 +1233,11 @@
       <c r="AN3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:40">
+      <c r="AO3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1289,8 +1307,11 @@
       <c r="AN4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:40">
+      <c r="AO4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1412,7 +1433,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:41">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1534,7 +1555,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:41">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1602,7 +1623,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:41">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1721,7 +1742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:41">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1840,7 +1861,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:41">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1908,7 +1929,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:41">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2027,7 +2048,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:41">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2146,7 +2167,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:41">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2214,7 +2235,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:41">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2333,7 +2354,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:41">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2452,7 +2473,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:41">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5064,10 +5085,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:XFD45"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5965,6 +5986,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="44" spans="1:15">
+      <c r="A44" t="s">
+        <v>138</v>
+      </c>
+      <c r="B44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" t="s">
+        <v>66</v>
+      </c>
+      <c r="E44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
refactor controls, filters, add forms (WIP)
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16440" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="145">
   <si>
     <t>text</t>
   </si>
@@ -452,6 +452,12 @@
   </si>
   <si>
     <t>org</t>
+  </si>
+  <si>
+    <t>Boolean true/false value</t>
+  </si>
+  <si>
+    <t>Boolean true/false value or no value</t>
   </si>
 </sst>
 </file>
@@ -824,36 +830,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+    <sheetView topLeftCell="AG1" workbookViewId="0">
       <selection activeCell="AM39" sqref="AM39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="8" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="24" customWidth="1"/>
-    <col min="35" max="35" width="23.5" customWidth="1"/>
-    <col min="36" max="36" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.33203125" customWidth="1"/>
+    <col min="35" max="35" width="23.42578125" customWidth="1"/>
+    <col min="36" max="36" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -975,7 +981,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:40">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1097,7 +1103,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:40">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1219,7 +1225,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1290,7 +1296,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1412,7 +1418,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1534,7 +1540,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1602,7 +1608,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1721,7 +1727,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1840,7 +1846,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1908,7 +1914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2027,7 +2033,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2146,7 +2152,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2214,7 +2220,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2333,7 +2339,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2452,7 +2458,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2520,7 +2526,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2588,7 +2594,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:39">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2707,7 +2713,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:39">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2826,7 +2832,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:39">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2894,7 +2900,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:39">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3013,7 +3019,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:39">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3129,7 +3135,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:39">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3194,7 +3200,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:39">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3310,7 +3316,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:39">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3426,7 +3432,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:39">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3491,7 +3497,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:39">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3607,7 +3613,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:39">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3723,7 +3729,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:39">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3788,7 +3794,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:39">
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3904,7 +3910,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:39">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4020,7 +4026,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:39">
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4085,7 +4091,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:39">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4201,7 +4207,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:39">
+    <row r="34" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4317,7 +4323,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:39">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4382,7 +4388,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:39">
+    <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4447,7 +4453,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:39">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4563,7 +4569,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:39">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4679,7 +4685,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:39">
+    <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4889,9 +4895,9 @@
       <selection activeCell="A7" sqref="A7:XFD50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -4899,7 +4905,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -4907,7 +4913,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -4915,7 +4921,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -4923,7 +4929,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -4931,7 +4937,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -4957,12 +4963,12 @@
       <selection activeCell="A5" sqref="A5:A100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -4973,7 +4979,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -4984,7 +4990,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -4992,7 +4998,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -5015,14 +5021,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5033,7 +5039,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -5044,7 +5050,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -5064,24 +5070,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5127,8 +5134,11 @@
       <c r="O1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5148,7 +5158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -5171,7 +5181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -5191,7 +5201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -5210,8 +5220,11 @@
       <c r="M5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="P5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -5230,8 +5243,11 @@
       <c r="M6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="P6" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -5251,7 +5267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -5271,7 +5287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -5291,7 +5307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -5308,7 +5324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -5325,7 +5341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -5345,7 +5361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -5365,7 +5381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -5382,7 +5398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -5402,7 +5418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -5419,7 +5435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -5442,7 +5458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -5462,7 +5478,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -5479,7 +5495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -5499,7 +5515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -5519,7 +5535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -5536,7 +5552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -5556,7 +5572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -5573,7 +5589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -5596,7 +5612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -5619,7 +5635,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -5636,7 +5652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -5653,7 +5669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -5679,7 +5695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -5705,7 +5721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>52</v>
       </c>
@@ -5728,7 +5744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -5748,7 +5764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -5768,7 +5784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -5785,7 +5801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -5802,7 +5818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -5819,7 +5835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -5842,7 +5858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -5862,7 +5878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>95</v>
       </c>
@@ -5882,7 +5898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>96</v>
       </c>
@@ -5902,7 +5918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -5922,7 +5938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -5942,7 +5958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>136</v>
       </c>

</xml_diff>

<commit_message>
fixed input file for attribute mapping
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="152">
   <si>
     <t>text</t>
   </si>
@@ -452,6 +452,33 @@
   </si>
   <si>
     <t>org</t>
+  </si>
+  <si>
+    <t>xcomputedint</t>
+  </si>
+  <si>
+    <t>expression</t>
+  </si>
+  <si>
+    <t>xcomputedxref</t>
+  </si>
+  <si>
+    <t>abstract</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>{Chromosome: xstring, Position: xint}</t>
+  </si>
+  <si>
+    <t>entity for the computed attributes</t>
+  </si>
+  <si>
+    <t>Chromosome</t>
+  </si>
+  <si>
+    <t>Position</t>
   </si>
 </sst>
 </file>
@@ -500,9 +527,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -515,13 +544,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="10">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -824,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AM39" sqref="AM39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5009,20 +5040,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5032,8 +5063,11 @@
       <c r="C1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -5044,7 +5078,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -5052,8 +5086,17 @@
         <v>138</v>
       </c>
     </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" t="s">
+        <v>149</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -5064,24 +5107,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD43"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5127,8 +5171,11 @@
       <c r="O1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5148,7 +5195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -5171,7 +5218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -5191,7 +5238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -5211,7 +5258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -5231,7 +5278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -5251,7 +5298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -5271,7 +5318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -5291,7 +5338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -5308,7 +5355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -5325,7 +5372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -5345,7 +5392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -5365,7 +5412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -5382,7 +5429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -5402,7 +5449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -5748,7 +5795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15">
+    <row r="33" spans="1:16">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -5768,7 +5815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15">
+    <row r="34" spans="1:16">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -5785,7 +5832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15">
+    <row r="35" spans="1:16">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -5802,7 +5849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15">
+    <row r="36" spans="1:16">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -5819,7 +5866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15">
+    <row r="37" spans="1:16">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -5842,7 +5889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15">
+    <row r="38" spans="1:16">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -5862,7 +5909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15">
+    <row r="39" spans="1:16">
       <c r="A39" t="s">
         <v>95</v>
       </c>
@@ -5882,7 +5929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15">
+    <row r="40" spans="1:16">
       <c r="A40" t="s">
         <v>96</v>
       </c>
@@ -5902,7 +5949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15">
+    <row r="41" spans="1:16">
       <c r="A41" t="s">
         <v>98</v>
       </c>
@@ -5922,7 +5969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:15">
+    <row r="42" spans="1:16">
       <c r="A42" t="s">
         <v>100</v>
       </c>
@@ -5942,7 +5989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:15">
+    <row r="43" spans="1:16">
       <c r="A43" t="s">
         <v>136</v>
       </c>
@@ -5963,6 +6010,89 @@
       </c>
       <c r="O43" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="A44" t="s">
+        <v>145</v>
+      </c>
+      <c r="B44" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" t="s">
+        <v>78</v>
+      </c>
+      <c r="D44" t="s">
+        <v>147</v>
+      </c>
+      <c r="E44" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
+      <c r="L44" t="b">
+        <v>1</v>
+      </c>
+      <c r="P44" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" t="s">
+        <v>143</v>
+      </c>
+      <c r="B45" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" t="b">
+        <v>0</v>
+      </c>
+      <c r="F45" t="b">
+        <v>1</v>
+      </c>
+      <c r="L45" t="b">
+        <v>1</v>
+      </c>
+      <c r="P45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="A46" t="s">
+        <v>150</v>
+      </c>
+      <c r="B46" t="s">
+        <v>147</v>
+      </c>
+      <c r="C46" t="s">
+        <v>66</v>
+      </c>
+      <c r="E46" t="b">
+        <v>0</v>
+      </c>
+      <c r="F46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" t="s">
+        <v>151</v>
+      </c>
+      <c r="B47" t="s">
+        <v>147</v>
+      </c>
+      <c r="C47" t="s">
+        <v>67</v>
+      </c>
+      <c r="E47" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new example test file
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="151">
   <si>
     <t>text</t>
   </si>
@@ -470,13 +470,19 @@
   </si>
   <si>
     <t>{Chromosome: xstring, Position: xint}</t>
+  </si>
+  <si>
+    <t>Chromosome</t>
+  </si>
+  <si>
+    <t>Position</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -496,6 +502,13 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -529,10 +542,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5029,10 +5043,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5073,6 +5087,11 @@
       </c>
       <c r="B3" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -5088,10 +5107,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P45" sqref="P45"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6042,6 +6061,62 @@
         <v>29</v>
       </c>
     </row>
+    <row r="46" spans="1:16">
+      <c r="A46" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F46" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="3"/>
+      <c r="P46" s="3"/>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="A47" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Refactor work in progress
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16440" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1737" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="173">
   <si>
     <t>text</t>
   </si>
@@ -539,6 +539,12 @@
 print(y)              # print (vector) y
 mean(y)               # Calculate average (arithmetic mean) of (vector) y; result is scalar
 var(y)                # Calculate sample variance</t>
+  </si>
+  <si>
+    <t>xintcomputed</t>
+  </si>
+  <si>
+    <t>expression</t>
   </si>
 </sst>
 </file>
@@ -914,9 +920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BK39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK39" workbookViewId="0">
-      <selection activeCell="AU2" sqref="AU2:AW39"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7891,10 +7895,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P66"/>
+  <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="M52" sqref="M52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7907,9 +7911,10 @@
     <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -7958,8 +7963,11 @@
       <c r="P1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -7979,7 +7987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -8002,7 +8010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -8022,7 +8030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -8045,7 +8053,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -8068,7 +8076,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>147</v>
       </c>
@@ -8094,7 +8102,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -8114,7 +8122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -8134,7 +8142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>148</v>
       </c>
@@ -8157,7 +8165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -8177,7 +8185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -8194,7 +8202,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>149</v>
       </c>
@@ -8217,7 +8225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -8234,7 +8242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -8254,7 +8262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>150</v>
       </c>
@@ -8600,7 +8608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -8617,7 +8625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>156</v>
       </c>
@@ -8640,7 +8648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -8663,7 +8671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -8686,7 +8694,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>157</v>
       </c>
@@ -8712,26 +8720,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>171</v>
       </c>
       <c r="B38" t="s">
         <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
       </c>
       <c r="F38" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
         <v>57</v>
@@ -8743,12 +8754,12 @@
         <v>0</v>
       </c>
       <c r="F39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>158</v>
+        <v>34</v>
       </c>
       <c r="B40" t="s">
         <v>57</v>
@@ -8760,15 +8771,12 @@
         <v>0</v>
       </c>
       <c r="F40" t="b">
-        <v>0</v>
-      </c>
-      <c r="L40" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>158</v>
       </c>
       <c r="B41" t="s">
         <v>57</v>
@@ -8782,19 +8790,13 @@
       <c r="F41" t="b">
         <v>0</v>
       </c>
-      <c r="H41">
-        <v>0</v>
-      </c>
-      <c r="I41">
-        <v>10</v>
-      </c>
-      <c r="M41" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B42" t="s">
         <v>57</v>
@@ -8806,7 +8808,7 @@
         <v>0</v>
       </c>
       <c r="F42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -8818,9 +8820,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>159</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
         <v>57</v>
@@ -8832,7 +8834,7 @@
         <v>0</v>
       </c>
       <c r="F43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -8840,25 +8842,19 @@
       <c r="I43">
         <v>10</v>
       </c>
-      <c r="L43" t="b">
-        <v>1</v>
-      </c>
       <c r="M43" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>52</v>
+        <v>159</v>
       </c>
       <c r="B44" t="s">
         <v>57</v>
       </c>
       <c r="C44" t="s">
-        <v>77</v>
-      </c>
-      <c r="D44" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="E44" t="b">
         <v>0</v>
@@ -8866,13 +8862,22 @@
       <c r="F44" t="b">
         <v>0</v>
       </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>10</v>
+      </c>
+      <c r="L44" t="b">
+        <v>1</v>
+      </c>
       <c r="M44" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>52</v>
       </c>
       <c r="B45" t="s">
         <v>57</v>
@@ -8887,12 +8892,15 @@
         <v>0</v>
       </c>
       <c r="F45" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="M45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>161</v>
+        <v>37</v>
       </c>
       <c r="B46" t="s">
         <v>57</v>
@@ -8907,24 +8915,18 @@
         <v>0</v>
       </c>
       <c r="F46" t="b">
-        <v>0</v>
-      </c>
-      <c r="L46" t="b">
-        <v>1</v>
-      </c>
-      <c r="M46" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="B47" t="s">
         <v>57</v>
       </c>
       <c r="C47" t="s">
-        <v>165</v>
+        <v>77</v>
       </c>
       <c r="D47" t="s">
         <v>59</v>
@@ -8935,13 +8937,16 @@
       <c r="F47" t="b">
         <v>0</v>
       </c>
+      <c r="L47" t="b">
+        <v>1</v>
+      </c>
       <c r="M47" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B48" t="s">
         <v>57</v>
@@ -8956,12 +8961,15 @@
         <v>0</v>
       </c>
       <c r="F48" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="M48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="B49" t="s">
         <v>57</v>
@@ -8976,24 +8984,21 @@
         <v>0</v>
       </c>
       <c r="F49" t="b">
-        <v>0</v>
-      </c>
-      <c r="L49" t="b">
-        <v>1</v>
-      </c>
-      <c r="M49" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B50" t="s">
         <v>57</v>
       </c>
       <c r="C50" t="s">
-        <v>169</v>
+        <v>165</v>
+      </c>
+      <c r="D50" t="s">
+        <v>59</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
@@ -9001,10 +9006,16 @@
       <c r="F50" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L50" t="b">
+        <v>1</v>
+      </c>
+      <c r="M50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B51" t="s">
         <v>57</v>
@@ -9016,12 +9027,12 @@
         <v>0</v>
       </c>
       <c r="F51" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B52" t="s">
         <v>57</v>
@@ -9033,21 +9044,18 @@
         <v>0</v>
       </c>
       <c r="F52" t="b">
-        <v>0</v>
-      </c>
-      <c r="L52" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>38</v>
+        <v>168</v>
       </c>
       <c r="B53" t="s">
         <v>57</v>
       </c>
       <c r="C53" t="s">
-        <v>66</v>
+        <v>169</v>
       </c>
       <c r="E53" t="b">
         <v>0</v>
@@ -9055,13 +9063,13 @@
       <c r="F53" t="b">
         <v>0</v>
       </c>
-      <c r="M53" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L53" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B54" t="s">
         <v>57</v>
@@ -9073,12 +9081,15 @@
         <v>0</v>
       </c>
       <c r="F54" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="M54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>162</v>
+        <v>39</v>
       </c>
       <c r="B55" t="s">
         <v>57</v>
@@ -9090,24 +9101,18 @@
         <v>0</v>
       </c>
       <c r="F55" t="b">
-        <v>0</v>
-      </c>
-      <c r="L55" t="b">
-        <v>1</v>
-      </c>
-      <c r="M55" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>40</v>
+        <v>162</v>
       </c>
       <c r="B56" t="s">
         <v>57</v>
       </c>
       <c r="C56" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="E56" t="b">
         <v>0</v>
@@ -9115,10 +9120,16 @@
       <c r="F56" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L56" t="b">
+        <v>1</v>
+      </c>
+      <c r="M56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B57" t="s">
         <v>57</v>
@@ -9130,12 +9141,12 @@
         <v>0</v>
       </c>
       <c r="F57" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>163</v>
+        <v>41</v>
       </c>
       <c r="B58" t="s">
         <v>57</v>
@@ -9147,24 +9158,18 @@
         <v>0</v>
       </c>
       <c r="F58" t="b">
-        <v>0</v>
-      </c>
-      <c r="L58" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>42</v>
+        <v>163</v>
       </c>
       <c r="B59" t="s">
         <v>57</v>
       </c>
       <c r="C59" t="s">
-        <v>78</v>
-      </c>
-      <c r="D59" t="s">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="E59" t="b">
         <v>0</v>
@@ -9172,13 +9177,13 @@
       <c r="F59" t="b">
         <v>0</v>
       </c>
-      <c r="M59" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B60" t="s">
         <v>57</v>
@@ -9193,12 +9198,15 @@
         <v>0</v>
       </c>
       <c r="F60" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="M60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>164</v>
+        <v>43</v>
       </c>
       <c r="B61" t="s">
         <v>57</v>
@@ -9213,24 +9221,21 @@
         <v>0</v>
       </c>
       <c r="F61" t="b">
-        <v>0</v>
-      </c>
-      <c r="L61" t="b">
-        <v>1</v>
-      </c>
-      <c r="M61" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>95</v>
+        <v>164</v>
       </c>
       <c r="B62" t="s">
         <v>57</v>
       </c>
       <c r="C62" t="s">
-        <v>66</v>
+        <v>78</v>
+      </c>
+      <c r="D62" t="s">
+        <v>59</v>
       </c>
       <c r="E62" t="b">
         <v>0</v>
@@ -9238,13 +9243,16 @@
       <c r="F62" t="b">
         <v>0</v>
       </c>
-      <c r="N62" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L62" t="b">
+        <v>1</v>
+      </c>
+      <c r="M62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B63" t="s">
         <v>57</v>
@@ -9256,15 +9264,15 @@
         <v>0</v>
       </c>
       <c r="F63" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N63" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B64" t="s">
         <v>57</v>
@@ -9276,21 +9284,21 @@
         <v>0</v>
       </c>
       <c r="F64" t="b">
-        <v>0</v>
-      </c>
-      <c r="O64" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="N64" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B65" t="s">
         <v>57</v>
       </c>
       <c r="C65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E65" t="b">
         <v>0</v>
@@ -9304,24 +9312,44 @@
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="B66" t="s">
         <v>57</v>
       </c>
       <c r="C66" t="s">
+        <v>67</v>
+      </c>
+      <c r="E66" t="b">
+        <v>0</v>
+      </c>
+      <c r="F66" t="b">
+        <v>0</v>
+      </c>
+      <c r="O66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>136</v>
+      </c>
+      <c r="B67" t="s">
+        <v>57</v>
+      </c>
+      <c r="C67" t="s">
         <v>78</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D67" t="s">
         <v>59</v>
       </c>
-      <c r="E66" t="b">
-        <v>0</v>
-      </c>
-      <c r="F66" t="b">
-        <v>1</v>
-      </c>
-      <c r="O66" t="b">
+      <c r="E67" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" t="b">
+        <v>1</v>
+      </c>
+      <c r="O67" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change the xcategorialmrefnillable_value column name to xcatmrefnillable_value due to upload problems (reference key created by mysql is too long).
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4935" yWindow="1665" windowWidth="25605" windowHeight="14625"/>
+    <workbookView xWindow="4940" yWindow="1660" windowWidth="25600" windowHeight="14620" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
@@ -502,7 +502,7 @@
     <t>xcategoricalmref_value</t>
   </si>
   <si>
-    <t>xcategoricalmrefnillable_value</t>
+    <t>xcatmrefnillable_value</t>
   </si>
 </sst>
 </file>
@@ -558,9 +558,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -576,7 +577,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -585,6 +586,7 @@
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -887,40 +889,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="20.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="8" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="24" customWidth="1"/>
-    <col min="39" max="39" width="23.42578125" customWidth="1"/>
-    <col min="40" max="40" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.28515625" customWidth="1"/>
+    <col min="39" max="39" width="23.5" customWidth="1"/>
+    <col min="40" max="40" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -1054,7 +1056,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1188,7 +1190,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1322,7 +1324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1402,7 +1404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1536,7 +1538,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1670,7 +1672,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1747,7 +1749,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1878,7 +1880,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2009,7 +2011,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2086,7 +2088,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2217,7 +2219,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2348,7 +2350,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2425,7 +2427,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2556,7 +2558,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2687,7 +2689,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2764,7 +2766,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2841,7 +2843,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2972,7 +2974,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3103,7 +3105,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3180,7 +3182,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3311,7 +3313,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3439,7 +3441,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3513,7 +3515,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3641,7 +3643,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3769,7 +3771,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3843,7 +3845,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:43">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3971,7 +3973,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4099,7 +4101,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4173,7 +4175,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4301,7 +4303,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4429,7 +4431,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4503,7 +4505,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4631,7 +4633,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4759,7 +4761,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4833,7 +4835,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:43">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4907,7 +4909,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:43">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5035,7 +5037,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:43">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5163,7 +5165,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:43">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5382,9 +5384,9 @@
       <selection activeCell="A7" sqref="A7:XFD50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -5392,7 +5394,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -5400,7 +5402,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -5408,7 +5410,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -5416,7 +5418,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -5424,7 +5426,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -5450,12 +5452,12 @@
       <selection activeCell="A5" sqref="A5:A100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5466,7 +5468,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -5477,7 +5479,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -5485,7 +5487,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -5508,14 +5510,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5529,7 +5531,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -5540,7 +5542,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -5548,7 +5550,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>147</v>
       </c>
@@ -5568,23 +5570,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5637,7 +5639,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5657,7 +5659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -5680,7 +5682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -5700,7 +5702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -5720,7 +5722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -5740,7 +5742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>151</v>
       </c>
@@ -5757,7 +5759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>153</v>
       </c>
@@ -5780,7 +5782,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>154</v>
       </c>
@@ -5803,7 +5805,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -5823,7 +5825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -5843,7 +5845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>158</v>
       </c>
@@ -5866,7 +5868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>159</v>
       </c>
@@ -5886,7 +5888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -5906,7 +5908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -5923,7 +5925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -5940,7 +5942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -5960,7 +5962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -5980,7 +5982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -5997,7 +5999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -6017,7 +6019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -6034,7 +6036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -6057,7 +6059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -6077,7 +6079,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -6094,7 +6096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -6114,7 +6116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -6134,7 +6136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -6151,7 +6153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -6171,7 +6173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -6188,7 +6190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -6211,7 +6213,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -6234,7 +6236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -6251,7 +6253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -6268,7 +6270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -6294,7 +6296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -6320,7 +6322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -6343,7 +6345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -6363,7 +6365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -6383,7 +6385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -6400,7 +6402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -6417,7 +6419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -6434,7 +6436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -6457,7 +6459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -6477,7 +6479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15">
       <c r="A44" t="s">
         <v>95</v>
       </c>
@@ -6497,7 +6499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -6517,7 +6519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15">
       <c r="A46" t="s">
         <v>98</v>
       </c>
@@ -6537,7 +6539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15">
       <c r="A47" t="s">
         <v>100</v>
       </c>
@@ -6557,7 +6559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15">
       <c r="A48" t="s">
         <v>136</v>
       </c>
@@ -6580,7 +6582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17">
       <c r="A49" t="s">
         <v>145</v>
       </c>
@@ -6606,7 +6608,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17">
       <c r="A50" t="s">
         <v>143</v>
       </c>
@@ -6629,7 +6631,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17">
       <c r="A51" s="3" t="s">
         <v>149</v>
       </c>
@@ -6658,7 +6660,7 @@
       <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17">
       <c r="A52" s="3" t="s">
         <v>150</v>
       </c>

</xml_diff>

<commit_message>
Added extra js methods to script evaluator
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="1660" windowWidth="25600" windowHeight="14620" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37420" windowHeight="21100" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="167">
   <si>
     <t>text</t>
   </si>
@@ -503,6 +503,27 @@
   </si>
   <si>
     <t>xcatmrefnillable_value</t>
+  </si>
+  <si>
+    <t>validationExpression</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>AUTO</t>
+  </si>
+  <si>
+    <t>driverslicence</t>
+  </si>
+  <si>
+    <t>$('age').ge(18).value()</t>
+  </si>
+  <si>
+    <t>$('driverslicence').isNull().not().or($('age').isNull()).or($('age').lt(18)).value()</t>
   </si>
 </sst>
 </file>
@@ -558,9 +579,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -577,7 +600,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -587,6 +610,8 @@
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -5568,10 +5593,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:R55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="R55" sqref="R55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5586,7 +5611,7 @@
     <col min="17" max="17" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5638,8 +5663,11 @@
       <c r="Q1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5659,7 +5687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -5682,7 +5710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -5702,7 +5730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -5722,7 +5750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -5742,7 +5770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>151</v>
       </c>
@@ -5759,7 +5787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>153</v>
       </c>
@@ -5782,7 +5810,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>154</v>
       </c>
@@ -5805,7 +5833,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -5825,7 +5853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -5845,7 +5873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>158</v>
       </c>
@@ -5868,7 +5896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>159</v>
       </c>
@@ -5888,7 +5916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -5908,7 +5936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -5925,7 +5953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -6582,7 +6610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:18">
       <c r="A49" t="s">
         <v>145</v>
       </c>
@@ -6608,7 +6636,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:18">
       <c r="A50" t="s">
         <v>143</v>
       </c>
@@ -6631,7 +6659,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:18">
       <c r="A51" s="3" t="s">
         <v>149</v>
       </c>
@@ -6660,7 +6688,7 @@
       <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
     </row>
-    <row r="52" spans="1:17">
+    <row r="52" spans="1:18">
       <c r="A52" s="3" t="s">
         <v>150</v>
       </c>
@@ -6684,10 +6712,67 @@
       <c r="K52" s="3"/>
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+    </row>
+    <row r="53" spans="1:18">
+      <c r="A53" t="s">
+        <v>60</v>
+      </c>
+      <c r="B53" t="s">
+        <v>162</v>
+      </c>
+      <c r="C53" t="s">
+        <v>66</v>
+      </c>
+      <c r="E53" t="s">
+        <v>163</v>
+      </c>
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18">
+      <c r="A54" t="s">
+        <v>161</v>
+      </c>
+      <c r="B54" t="s">
+        <v>162</v>
+      </c>
+      <c r="C54" t="s">
+        <v>67</v>
+      </c>
+      <c r="E54" t="b">
+        <v>0</v>
+      </c>
+      <c r="F54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18">
+      <c r="A55" t="s">
+        <v>164</v>
+      </c>
+      <c r="B55" t="s">
+        <v>162</v>
+      </c>
+      <c r="C55" t="s">
+        <v>68</v>
+      </c>
+      <c r="E55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" t="b">
+        <v>1</v>
+      </c>
+      <c r="N55" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="R55" t="s">
+        <v>166</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Use full entity names in EMX file
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="1660" windowWidth="25600" windowHeight="14620" activeTab="4"/>
+    <workbookView xWindow="4980" yWindow="1660" windowWidth="25600" windowHeight="16740" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
-    <sheet name="TypeTestRef" sheetId="2" r:id="rId2"/>
+    <sheet name="org_molgenis_test_TypeTest" sheetId="1" r:id="rId1"/>
+    <sheet name="org_molgenis_test_TypeTestRef" sheetId="2" r:id="rId2"/>
     <sheet name="packages" sheetId="5" r:id="rId3"/>
     <sheet name="entities" sheetId="3" r:id="rId4"/>
     <sheet name="attributes" sheetId="4" r:id="rId5"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="162">
   <si>
     <t>text</t>
   </si>
@@ -439,18 +439,12 @@
     <t>parent</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>Molgenis test package</t>
   </si>
   <si>
     <t>package</t>
   </si>
   <si>
-    <t>molgenis</t>
-  </si>
-  <si>
     <t>org</t>
   </si>
   <si>
@@ -503,6 +497,18 @@
   </si>
   <si>
     <t>xcatmrefnillable_value</t>
+  </si>
+  <si>
+    <t>org_molgenis</t>
+  </si>
+  <si>
+    <t>org_molgenis_test</t>
+  </si>
+  <si>
+    <t>org_molgenis_test_TypeTestRef</t>
+  </si>
+  <si>
+    <t>org_molgenis_test_TypeTest</t>
   </si>
 </sst>
 </file>
@@ -558,9 +564,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -577,7 +586,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="14">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -587,6 +596,9 @@
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -933,10 +945,10 @@
         <v>45</v>
       </c>
       <c r="D1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F1" t="s">
         <v>46</v>
@@ -945,10 +957,10 @@
         <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J1" t="s">
         <v>20</v>
@@ -1070,7 +1082,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F2" t="s">
         <v>2</v>
@@ -1204,7 +1216,7 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
@@ -1335,7 +1347,7 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F4" t="s">
         <v>4</v>
@@ -1418,7 +1430,7 @@
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F5" t="s">
         <v>2</v>
@@ -1552,7 +1564,7 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F6" t="s">
         <v>3</v>
@@ -1683,7 +1695,7 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F7" t="s">
         <v>4</v>
@@ -1763,7 +1775,7 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F8" t="s">
         <v>2</v>
@@ -1894,7 +1906,7 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F9" t="s">
         <v>3</v>
@@ -2022,7 +2034,7 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F10" t="s">
         <v>4</v>
@@ -2102,7 +2114,7 @@
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F11" t="s">
         <v>2</v>
@@ -2233,7 +2245,7 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F12" t="s">
         <v>3</v>
@@ -2361,7 +2373,7 @@
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F13" t="s">
         <v>4</v>
@@ -2441,7 +2453,7 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F14" t="s">
         <v>2</v>
@@ -2572,7 +2584,7 @@
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F15" t="s">
         <v>3</v>
@@ -2700,7 +2712,7 @@
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F16" t="s">
         <v>4</v>
@@ -2777,7 +2789,7 @@
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F17" t="s">
         <v>4</v>
@@ -2857,7 +2869,7 @@
         <v>17</v>
       </c>
       <c r="E18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F18" t="s">
         <v>2</v>
@@ -2988,7 +3000,7 @@
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F19" t="s">
         <v>3</v>
@@ -3116,7 +3128,7 @@
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F20" t="s">
         <v>4</v>
@@ -3196,7 +3208,7 @@
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F21" t="s">
         <v>2</v>
@@ -3327,7 +3339,7 @@
         <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F22" t="s">
         <v>3</v>
@@ -3452,7 +3464,7 @@
         <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F23" t="s">
         <v>4</v>
@@ -3529,7 +3541,7 @@
         <v>23</v>
       </c>
       <c r="E24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F24" t="s">
         <v>2</v>
@@ -3657,7 +3669,7 @@
         <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F25" t="s">
         <v>3</v>
@@ -3782,7 +3794,7 @@
         <v>25</v>
       </c>
       <c r="E26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F26" t="s">
         <v>4</v>
@@ -3859,7 +3871,7 @@
         <v>26</v>
       </c>
       <c r="E27" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F27" t="s">
         <v>2</v>
@@ -3987,7 +3999,7 @@
         <v>27</v>
       </c>
       <c r="E28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F28" t="s">
         <v>3</v>
@@ -4112,7 +4124,7 @@
         <v>28</v>
       </c>
       <c r="E29" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F29" t="s">
         <v>4</v>
@@ -4189,7 +4201,7 @@
         <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F30" t="s">
         <v>2</v>
@@ -4317,7 +4329,7 @@
         <v>30</v>
       </c>
       <c r="E31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F31" t="s">
         <v>3</v>
@@ -4442,7 +4454,7 @@
         <v>31</v>
       </c>
       <c r="E32" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F32" t="s">
         <v>4</v>
@@ -4519,7 +4531,7 @@
         <v>32</v>
       </c>
       <c r="E33" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F33" t="s">
         <v>2</v>
@@ -4647,7 +4659,7 @@
         <v>33</v>
       </c>
       <c r="E34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F34" t="s">
         <v>3</v>
@@ -4772,7 +4784,7 @@
         <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F35" t="s">
         <v>4</v>
@@ -4846,7 +4858,7 @@
         <v>35</v>
       </c>
       <c r="E36" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F36" t="s">
         <v>4</v>
@@ -4923,7 +4935,7 @@
         <v>36</v>
       </c>
       <c r="E37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F37" t="s">
         <v>2</v>
@@ -5051,7 +5063,7 @@
         <v>37</v>
       </c>
       <c r="E38" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F38" t="s">
         <v>3</v>
@@ -5176,7 +5188,7 @@
         <v>38</v>
       </c>
       <c r="E39" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F39" t="s">
         <v>4</v>
@@ -5381,7 +5393,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD50"/>
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5448,12 +5460,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A100"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5470,26 +5483,26 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" t="s">
         <v>138</v>
       </c>
-      <c r="B2" t="s">
-        <v>139</v>
-      </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -5507,13 +5520,13 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5522,13 +5535,13 @@
         <v>55</v>
       </c>
       <c r="B1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C1" t="s">
         <v>56</v>
       </c>
       <c r="D1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -5536,7 +5549,7 @@
         <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="C2" t="s">
         <v>58</v>
@@ -5547,12 +5560,12 @@
         <v>59</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -5570,16 +5583,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
@@ -5633,10 +5646,10 @@
         <v>99</v>
       </c>
       <c r="P1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="Q1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -5644,7 +5657,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="C2" t="s">
         <v>66</v>
@@ -5664,7 +5677,7 @@
         <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="C3" t="s">
         <v>66</v>
@@ -5687,7 +5700,7 @@
         <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C4" t="s">
         <v>67</v>
@@ -5707,7 +5720,7 @@
         <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C5" t="s">
         <v>68</v>
@@ -5727,7 +5740,7 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
         <v>68</v>
@@ -5744,13 +5757,13 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -5761,10 +5774,10 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C8" t="s">
         <v>67</v>
@@ -5779,15 +5792,15 @@
         <v>1</v>
       </c>
       <c r="P8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C9" t="s">
         <v>66</v>
@@ -5802,7 +5815,7 @@
         <v>1</v>
       </c>
       <c r="P9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -5810,13 +5823,13 @@
         <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C10" t="s">
         <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -5830,13 +5843,13 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C11" t="s">
         <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -5847,16 +5860,16 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -5870,16 +5883,16 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B13" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D13" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -5893,7 +5906,7 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C14" t="s">
         <v>70</v>
@@ -5913,7 +5926,7 @@
         <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C15" t="s">
         <v>70</v>
@@ -5930,7 +5943,7 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C16" t="s">
         <v>71</v>
@@ -5947,7 +5960,7 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C17" t="s">
         <v>71</v>
@@ -5967,7 +5980,7 @@
         <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C18" t="s">
         <v>72</v>
@@ -5987,7 +6000,7 @@
         <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C19" t="s">
         <v>72</v>
@@ -6004,7 +6017,7 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C20" t="s">
         <v>73</v>
@@ -6024,7 +6037,7 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C21" t="s">
         <v>73</v>
@@ -6041,7 +6054,7 @@
         <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C22" t="s">
         <v>80</v>
@@ -6064,7 +6077,7 @@
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C23" t="s">
         <v>80</v>
@@ -6084,7 +6097,7 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C24" t="s">
         <v>74</v>
@@ -6101,7 +6114,7 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C25" t="s">
         <v>74</v>
@@ -6121,7 +6134,7 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C26" t="s">
         <v>75</v>
@@ -6141,7 +6154,7 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C27" t="s">
         <v>75</v>
@@ -6158,7 +6171,7 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C28" t="s">
         <v>67</v>
@@ -6178,7 +6191,7 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C29" t="s">
         <v>67</v>
@@ -6195,7 +6208,7 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C30" t="s">
         <v>67</v>
@@ -6218,7 +6231,7 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C31" t="s">
         <v>67</v>
@@ -6241,7 +6254,7 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C32" t="s">
         <v>76</v>
@@ -6258,7 +6271,7 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C33" t="s">
         <v>76</v>
@@ -6275,7 +6288,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C34" t="s">
         <v>76</v>
@@ -6301,7 +6314,7 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C35" t="s">
         <v>76</v>
@@ -6327,13 +6340,13 @@
         <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C36" t="s">
         <v>77</v>
       </c>
       <c r="D36" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -6350,13 +6363,13 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C37" t="s">
         <v>77</v>
       </c>
       <c r="D37" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
@@ -6370,7 +6383,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C38" t="s">
         <v>66</v>
@@ -6390,7 +6403,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C39" t="s">
         <v>66</v>
@@ -6407,7 +6420,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C40" t="s">
         <v>0</v>
@@ -6424,7 +6437,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C41" t="s">
         <v>0</v>
@@ -6441,13 +6454,13 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C42" t="s">
         <v>78</v>
       </c>
       <c r="D42" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
@@ -6464,13 +6477,13 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C43" t="s">
         <v>78</v>
       </c>
       <c r="D43" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
@@ -6484,7 +6497,7 @@
         <v>95</v>
       </c>
       <c r="B44" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C44" t="s">
         <v>66</v>
@@ -6504,7 +6517,7 @@
         <v>96</v>
       </c>
       <c r="B45" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C45" t="s">
         <v>66</v>
@@ -6524,7 +6537,7 @@
         <v>98</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C46" t="s">
         <v>66</v>
@@ -6544,7 +6557,7 @@
         <v>100</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C47" t="s">
         <v>67</v>
@@ -6564,13 +6577,13 @@
         <v>136</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C48" t="s">
         <v>78</v>
       </c>
       <c r="D48" t="s">
-        <v>59</v>
+        <v>160</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
@@ -6584,16 +6597,16 @@
     </row>
     <row r="49" spans="1:17">
       <c r="A49" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C49" t="s">
         <v>78</v>
       </c>
       <c r="D49" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -6605,15 +6618,15 @@
         <v>1</v>
       </c>
       <c r="Q49" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:17">
       <c r="A50" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B50" t="s">
-        <v>57</v>
+        <v>161</v>
       </c>
       <c r="C50" t="s">
         <v>67</v>
@@ -6633,10 +6646,10 @@
     </row>
     <row r="51" spans="1:17">
       <c r="A51" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>66</v>
@@ -6662,10 +6675,10 @@
     </row>
     <row r="52" spans="1:17">
       <c r="A52" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Added packages tab to importer
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4980" yWindow="1660" windowWidth="25600" windowHeight="16740" activeTab="2"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="31020" windowHeight="18480" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="org_molgenis_test_TypeTest" sheetId="1" r:id="rId1"/>
+    <sheet name="TypeTest" sheetId="1" r:id="rId1"/>
     <sheet name="org_molgenis_test_TypeTestRef" sheetId="2" r:id="rId2"/>
     <sheet name="packages" sheetId="5" r:id="rId3"/>
     <sheet name="entities" sheetId="3" r:id="rId4"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="161">
   <si>
     <t>text</t>
   </si>
@@ -506,9 +506,6 @@
   </si>
   <si>
     <t>org_molgenis_test_TypeTestRef</t>
-  </si>
-  <si>
-    <t>org_molgenis_test_TypeTest</t>
   </si>
 </sst>
 </file>
@@ -564,9 +561,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -586,7 +586,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -599,6 +599,9 @@
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -5393,7 +5396,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5460,7 +5463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -5520,7 +5523,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5547,9 +5550,6 @@
     <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>57</v>
-      </c>
-      <c r="B2" t="s">
-        <v>159</v>
       </c>
       <c r="C2" t="s">
         <v>58</v>
@@ -5583,8 +5583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5700,7 +5700,7 @@
         <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
         <v>67</v>
@@ -5720,7 +5720,7 @@
         <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
         <v>68</v>
@@ -5740,7 +5740,7 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
         <v>68</v>
@@ -5760,7 +5760,7 @@
         <v>149</v>
       </c>
       <c r="B7" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
         <v>150</v>
@@ -5777,7 +5777,7 @@
         <v>151</v>
       </c>
       <c r="B8" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
         <v>67</v>
@@ -5800,7 +5800,7 @@
         <v>152</v>
       </c>
       <c r="B9" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
         <v>66</v>
@@ -5823,7 +5823,7 @@
         <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
         <v>69</v>
@@ -5843,7 +5843,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
         <v>69</v>
@@ -5863,7 +5863,7 @@
         <v>156</v>
       </c>
       <c r="B12" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
         <v>155</v>
@@ -5886,7 +5886,7 @@
         <v>157</v>
       </c>
       <c r="B13" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
         <v>155</v>
@@ -5906,7 +5906,7 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
         <v>70</v>
@@ -5926,7 +5926,7 @@
         <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
         <v>70</v>
@@ -5943,7 +5943,7 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
         <v>71</v>
@@ -5960,7 +5960,7 @@
         <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
         <v>71</v>
@@ -5980,7 +5980,7 @@
         <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
         <v>72</v>
@@ -6000,7 +6000,7 @@
         <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
         <v>72</v>
@@ -6017,7 +6017,7 @@
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
         <v>73</v>
@@ -6037,7 +6037,7 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
         <v>73</v>
@@ -6054,7 +6054,7 @@
         <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
         <v>80</v>
@@ -6077,7 +6077,7 @@
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
         <v>80</v>
@@ -6097,7 +6097,7 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
         <v>74</v>
@@ -6114,7 +6114,7 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
         <v>74</v>
@@ -6134,7 +6134,7 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
         <v>75</v>
@@ -6154,7 +6154,7 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s">
         <v>75</v>
@@ -6171,7 +6171,7 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
         <v>67</v>
@@ -6191,7 +6191,7 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
         <v>67</v>
@@ -6208,7 +6208,7 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
         <v>67</v>
@@ -6231,7 +6231,7 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
         <v>67</v>
@@ -6254,7 +6254,7 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C32" t="s">
         <v>76</v>
@@ -6271,7 +6271,7 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
         <v>76</v>
@@ -6288,7 +6288,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
         <v>76</v>
@@ -6314,7 +6314,7 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
         <v>76</v>
@@ -6340,12 +6340,12 @@
         <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C36" t="s">
         <v>77</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="3" t="s">
         <v>160</v>
       </c>
       <c r="E36" t="b">
@@ -6363,12 +6363,12 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C37" t="s">
         <v>77</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="3" t="s">
         <v>160</v>
       </c>
       <c r="E37" t="b">
@@ -6383,7 +6383,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
         <v>66</v>
@@ -6403,7 +6403,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C39" t="s">
         <v>66</v>
@@ -6420,7 +6420,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C40" t="s">
         <v>0</v>
@@ -6437,7 +6437,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C41" t="s">
         <v>0</v>
@@ -6454,12 +6454,12 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C42" t="s">
         <v>78</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="3" t="s">
         <v>160</v>
       </c>
       <c r="E42" t="b">
@@ -6477,12 +6477,12 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C43" t="s">
         <v>78</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="3" t="s">
         <v>160</v>
       </c>
       <c r="E43" t="b">
@@ -6497,7 +6497,7 @@
         <v>95</v>
       </c>
       <c r="B44" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C44" t="s">
         <v>66</v>
@@ -6517,7 +6517,7 @@
         <v>96</v>
       </c>
       <c r="B45" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C45" t="s">
         <v>66</v>
@@ -6537,7 +6537,7 @@
         <v>98</v>
       </c>
       <c r="B46" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C46" t="s">
         <v>66</v>
@@ -6557,7 +6557,7 @@
         <v>100</v>
       </c>
       <c r="B47" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C47" t="s">
         <v>67</v>
@@ -6577,12 +6577,12 @@
         <v>136</v>
       </c>
       <c r="B48" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C48" t="s">
         <v>78</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="3" t="s">
         <v>160</v>
       </c>
       <c r="E48" t="b">
@@ -6600,7 +6600,7 @@
         <v>143</v>
       </c>
       <c r="B49" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C49" t="s">
         <v>78</v>
@@ -6626,7 +6626,7 @@
         <v>141</v>
       </c>
       <c r="B50" t="s">
-        <v>161</v>
+        <v>57</v>
       </c>
       <c r="C50" t="s">
         <v>67</v>

</xml_diff>

<commit_message>
Add description to test dataset
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1144" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="160">
   <si>
     <t>text</t>
   </si>
@@ -558,9 +558,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -577,7 +578,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -587,6 +588,7 @@
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -5568,10 +5570,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:R52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5582,11 +5584,12 @@
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5609,37 +5612,40 @@
         <v>79</v>
       </c>
       <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
         <v>82</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>83</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>84</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>91</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>92</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>93</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>94</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>99</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>156</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5655,11 +5661,14 @@
       <c r="F2" t="b">
         <v>0</v>
       </c>
-      <c r="J2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -5675,14 +5684,17 @@
       <c r="F3" t="b">
         <v>0</v>
       </c>
-      <c r="J3" t="b">
-        <v>1</v>
+      <c r="H3" t="s">
+        <v>85</v>
       </c>
       <c r="K3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -5698,11 +5710,14 @@
       <c r="F4" t="b">
         <v>0</v>
       </c>
-      <c r="L4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="H4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -5718,11 +5733,14 @@
       <c r="F5" t="b">
         <v>0</v>
       </c>
-      <c r="M5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="N5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -5738,11 +5756,14 @@
       <c r="F6" t="b">
         <v>1</v>
       </c>
-      <c r="M6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="H6" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>151</v>
       </c>
@@ -5758,8 +5779,11 @@
       <c r="F7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="H7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>153</v>
       </c>
@@ -5775,14 +5799,17 @@
       <c r="F8" t="b">
         <v>1</v>
       </c>
-      <c r="M8" t="b">
-        <v>1</v>
-      </c>
-      <c r="P8" t="s">
+      <c r="H8" t="s">
+        <v>153</v>
+      </c>
+      <c r="N8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>154</v>
       </c>
@@ -5798,14 +5825,17 @@
       <c r="F9" t="b">
         <v>1</v>
       </c>
-      <c r="M9" t="b">
-        <v>1</v>
-      </c>
-      <c r="P9" t="s">
+      <c r="H9" t="s">
+        <v>154</v>
+      </c>
+      <c r="N9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -5824,8 +5854,11 @@
       <c r="F10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="H10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -5844,8 +5877,11 @@
       <c r="F11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>158</v>
       </c>
@@ -5864,11 +5900,14 @@
       <c r="F12" t="b">
         <v>0</v>
       </c>
-      <c r="M12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="H12" t="s">
+        <v>158</v>
+      </c>
+      <c r="N12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>159</v>
       </c>
@@ -5887,8 +5926,11 @@
       <c r="F13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="H13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -5904,11 +5946,14 @@
       <c r="F14" t="b">
         <v>0</v>
       </c>
-      <c r="M14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -5924,8 +5969,11 @@
       <c r="F15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="H15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -5941,8 +5989,11 @@
       <c r="F16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="H16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -5958,11 +6009,14 @@
       <c r="F17" t="b">
         <v>1</v>
       </c>
-      <c r="M17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="H17" t="s">
+        <v>21</v>
+      </c>
+      <c r="N17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -5978,11 +6032,14 @@
       <c r="F18" t="b">
         <v>0</v>
       </c>
-      <c r="M18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="H18" t="s">
+        <v>48</v>
+      </c>
+      <c r="N18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -5998,8 +6055,11 @@
       <c r="F19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="H19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -6015,11 +6075,14 @@
       <c r="F20" t="b">
         <v>0</v>
       </c>
-      <c r="M20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="H20" t="s">
+        <v>23</v>
+      </c>
+      <c r="N20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -6035,8 +6098,11 @@
       <c r="F21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="H21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -6055,11 +6121,14 @@
       <c r="G22" t="s">
         <v>81</v>
       </c>
-      <c r="M22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="H22" t="s">
+        <v>50</v>
+      </c>
+      <c r="N22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -6078,8 +6147,11 @@
       <c r="G23" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="H23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -6095,8 +6167,11 @@
       <c r="F24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:13">
+      <c r="H24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -6112,11 +6187,14 @@
       <c r="F25" t="b">
         <v>1</v>
       </c>
-      <c r="M25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13">
+      <c r="H25" t="s">
+        <v>26</v>
+      </c>
+      <c r="N25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -6132,11 +6210,14 @@
       <c r="F26" t="b">
         <v>0</v>
       </c>
-      <c r="M26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="H26" t="s">
+        <v>27</v>
+      </c>
+      <c r="N26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -6152,8 +6233,11 @@
       <c r="F27" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="H27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -6169,11 +6253,14 @@
       <c r="F28" t="b">
         <v>0</v>
       </c>
-      <c r="M28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="H28" t="s">
+        <v>29</v>
+      </c>
+      <c r="N28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -6189,8 +6276,11 @@
       <c r="F29" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="H29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -6206,14 +6296,17 @@
       <c r="F30" t="b">
         <v>0</v>
       </c>
-      <c r="H30">
-        <v>0</v>
+      <c r="H30" t="s">
+        <v>31</v>
       </c>
       <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -6229,14 +6322,17 @@
       <c r="F31" t="b">
         <v>1</v>
       </c>
-      <c r="H31">
-        <v>0</v>
+      <c r="H31" t="s">
+        <v>32</v>
       </c>
       <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -6252,8 +6348,11 @@
       <c r="F32" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="H32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -6269,8 +6368,11 @@
       <c r="F33" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="H33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -6286,17 +6388,20 @@
       <c r="F34" t="b">
         <v>0</v>
       </c>
-      <c r="H34">
-        <v>0</v>
+      <c r="H34" t="s">
+        <v>35</v>
       </c>
       <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
         <v>10</v>
       </c>
-      <c r="M34" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="N34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -6312,17 +6417,20 @@
       <c r="F35" t="b">
         <v>1</v>
       </c>
-      <c r="H35">
-        <v>0</v>
+      <c r="H35" t="s">
+        <v>36</v>
       </c>
       <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
         <v>10</v>
       </c>
-      <c r="M35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="N35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -6341,11 +6449,14 @@
       <c r="F36" t="b">
         <v>0</v>
       </c>
-      <c r="M36" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="H36" t="s">
+        <v>52</v>
+      </c>
+      <c r="N36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -6364,8 +6475,11 @@
       <c r="F37" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:15">
+      <c r="H37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -6381,11 +6495,14 @@
       <c r="F38" t="b">
         <v>0</v>
       </c>
-      <c r="M38" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15">
+      <c r="H38" t="s">
+        <v>38</v>
+      </c>
+      <c r="N38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -6401,8 +6518,11 @@
       <c r="F39" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="H39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -6418,8 +6538,11 @@
       <c r="F40" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:15">
+      <c r="H40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -6435,8 +6558,11 @@
       <c r="F41" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:15">
+      <c r="H41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -6455,11 +6581,14 @@
       <c r="F42" t="b">
         <v>0</v>
       </c>
-      <c r="M42" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15">
+      <c r="H42" t="s">
+        <v>42</v>
+      </c>
+      <c r="N42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -6478,8 +6607,11 @@
       <c r="F43" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:15">
+      <c r="H43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
       <c r="A44" t="s">
         <v>95</v>
       </c>
@@ -6495,11 +6627,14 @@
       <c r="F44" t="b">
         <v>0</v>
       </c>
-      <c r="N44" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15">
+      <c r="H44" t="s">
+        <v>95</v>
+      </c>
+      <c r="O44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -6515,11 +6650,14 @@
       <c r="F45" t="b">
         <v>1</v>
       </c>
-      <c r="N45" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15">
+      <c r="H45" t="s">
+        <v>96</v>
+      </c>
+      <c r="O45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
       <c r="A46" t="s">
         <v>98</v>
       </c>
@@ -6535,11 +6673,14 @@
       <c r="F46" t="b">
         <v>0</v>
       </c>
-      <c r="O46" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15">
+      <c r="H46" t="s">
+        <v>98</v>
+      </c>
+      <c r="P46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
       <c r="A47" t="s">
         <v>100</v>
       </c>
@@ -6555,11 +6696,14 @@
       <c r="F47" t="b">
         <v>0</v>
       </c>
-      <c r="O47" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15">
+      <c r="H47" t="s">
+        <v>100</v>
+      </c>
+      <c r="P47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
       <c r="A48" t="s">
         <v>136</v>
       </c>
@@ -6578,11 +6722,14 @@
       <c r="F48" t="b">
         <v>1</v>
       </c>
-      <c r="O48" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17">
+      <c r="H48" t="s">
+        <v>136</v>
+      </c>
+      <c r="P48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18">
       <c r="A49" t="s">
         <v>145</v>
       </c>
@@ -6601,14 +6748,17 @@
       <c r="F49" t="b">
         <v>1</v>
       </c>
-      <c r="L49" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q49" t="s">
+      <c r="H49" t="s">
+        <v>145</v>
+      </c>
+      <c r="M49" t="b">
+        <v>1</v>
+      </c>
+      <c r="R49" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:18">
       <c r="A50" t="s">
         <v>143</v>
       </c>
@@ -6624,14 +6774,17 @@
       <c r="F50" t="b">
         <v>1</v>
       </c>
-      <c r="L50" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q50" t="s">
+      <c r="H50" t="s">
+        <v>143</v>
+      </c>
+      <c r="M50" t="b">
+        <v>1</v>
+      </c>
+      <c r="R50" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:18">
       <c r="A51" s="3" t="s">
         <v>149</v>
       </c>
@@ -6649,7 +6802,9 @@
         <v>0</v>
       </c>
       <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
+      <c r="H51" s="3" t="s">
+        <v>149</v>
+      </c>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
@@ -6659,8 +6814,9 @@
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
-    </row>
-    <row r="52" spans="1:17">
+      <c r="R51" s="3"/>
+    </row>
+    <row r="52" spans="1:18">
       <c r="A52" s="3" t="s">
         <v>150</v>
       </c>
@@ -6678,7 +6834,9 @@
         <v>0</v>
       </c>
       <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
+      <c r="H52" s="3" t="s">
+        <v>150</v>
+      </c>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
@@ -6688,6 +6846,7 @@
       <c r="O52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removed emx_comp_test and reset emx_all_datatypes
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="345" windowWidth="31605" windowHeight="19200"/>
+    <workbookView xWindow="165" yWindow="345" windowWidth="22890" windowHeight="11070" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="org_molgenis_test_TypeTest" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="entities" sheetId="3" r:id="rId4"/>
     <sheet name="attributes" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -605,20 +605,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="14">
-    <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="5" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="7" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="9" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="11" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Gevolgde hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -919,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5412,7 +5412,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="A7" sqref="A7:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5599,8 +5599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6678,7 +6678,6 @@
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
       <c r="L51" s="3"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
@@ -6707,7 +6706,9 @@
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
+      <c r="K52" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="L52" s="3"/>
       <c r="M52" s="3"/>
       <c r="O52" s="3"/>

</xml_diff>

<commit_message>
Check all datatypes with defaultValue and get them to work.
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="165" yWindow="345" windowWidth="22890" windowHeight="11070" activeTab="4"/>
+    <workbookView xWindow="160" yWindow="340" windowWidth="36220" windowHeight="17880" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="org_molgenis_test_TypeTest" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1156" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="178">
   <si>
     <t>text</t>
   </si>
@@ -527,6 +527,36 @@
   </si>
   <si>
     <t>org_molgenis_test_TypeTest</t>
+  </si>
+  <si>
+    <t>defaultValue</t>
+  </si>
+  <si>
+    <t>typeTestRef</t>
+  </si>
+  <si>
+    <t>typeTestRefLabel</t>
+  </si>
+  <si>
+    <t>ref1,ref2</t>
+  </si>
+  <si>
+    <t>ref1,ref3</t>
+  </si>
+  <si>
+    <t>test@x.y.z</t>
+  </si>
+  <si>
+    <t>&lt;h1&gt;html 2&lt;/h1&gt;</t>
+  </si>
+  <si>
+    <t>http://www.nu.nl/</t>
+  </si>
+  <si>
+    <t>http://www.github.com/</t>
+  </si>
+  <si>
+    <t>xstringhidden</t>
   </si>
 </sst>
 </file>
@@ -582,7 +612,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -597,14 +627,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -617,6 +649,7 @@
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -920,40 +953,40 @@
   <dimension ref="A1:AR39"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="24" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="20.5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.28515625" customWidth="1"/>
-    <col min="33" max="33" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.33203125" customWidth="1"/>
+    <col min="33" max="33" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="8" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="24" customWidth="1"/>
-    <col min="39" max="39" width="23.42578125" customWidth="1"/>
-    <col min="40" max="40" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.28515625" customWidth="1"/>
+    <col min="39" max="39" width="23.5" customWidth="1"/>
+    <col min="40" max="40" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44">
       <c r="A1" t="s">
         <v>60</v>
       </c>
@@ -1087,7 +1120,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1221,7 +1254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1355,7 +1388,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1435,7 +1468,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1569,7 +1602,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1703,7 +1736,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1780,7 +1813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1911,7 +1944,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2042,7 +2075,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2119,7 +2152,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2250,7 +2283,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2381,7 +2414,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2458,7 +2491,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2589,7 +2622,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2720,7 +2753,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2797,7 +2830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2874,7 +2907,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3005,7 +3038,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3136,7 +3169,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:43">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3213,7 +3246,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3344,7 +3377,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:43">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3472,7 +3505,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:43">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3546,7 +3579,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:43">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3674,7 +3707,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:43">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3802,7 +3835,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:43">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3876,7 +3909,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:43">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4004,7 +4037,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4132,7 +4165,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4206,7 +4239,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4334,7 +4367,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4462,7 +4495,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:43">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4536,7 +4569,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:43">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4664,7 +4697,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4792,7 +4825,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:43">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4866,7 +4899,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:43">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4940,7 +4973,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:43">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5068,7 +5101,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:43">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5196,7 +5229,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:43">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5415,9 +5448,9 @@
       <selection activeCell="A7" sqref="A7:XFD50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -5425,7 +5458,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -5433,7 +5466,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -5441,7 +5474,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -5449,7 +5482,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -5457,7 +5490,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -5483,13 +5516,13 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5500,7 +5533,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>166</v>
       </c>
@@ -5511,7 +5544,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>165</v>
       </c>
@@ -5519,7 +5552,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -5542,14 +5575,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5563,7 +5596,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -5574,12 +5607,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -5597,25 +5630,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R55"/>
+  <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>55</v>
       </c>
@@ -5638,40 +5672,43 @@
         <v>79</v>
       </c>
       <c r="H1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" t="s">
         <v>82</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>83</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>84</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>91</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>92</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>93</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>94</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>99</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>154</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>142</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -5687,11 +5724,14 @@
       <c r="F2" t="b">
         <v>0</v>
       </c>
-      <c r="J2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -5707,14 +5747,17 @@
       <c r="F3" t="b">
         <v>0</v>
       </c>
-      <c r="J3" t="b">
-        <v>1</v>
+      <c r="H3" t="s">
+        <v>170</v>
       </c>
       <c r="K3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -5730,11 +5773,11 @@
       <c r="F4" t="b">
         <v>0</v>
       </c>
-      <c r="L4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -5750,11 +5793,14 @@
       <c r="F5" t="b">
         <v>0</v>
       </c>
-      <c r="M5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -5770,11 +5816,14 @@
       <c r="F6" t="b">
         <v>1</v>
       </c>
-      <c r="M6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>149</v>
       </c>
@@ -5791,7 +5840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19">
       <c r="A8" t="s">
         <v>151</v>
       </c>
@@ -5807,14 +5856,17 @@
       <c r="F8" t="b">
         <v>1</v>
       </c>
-      <c r="M8" t="b">
-        <v>1</v>
-      </c>
-      <c r="P8" t="s">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="N8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19">
       <c r="A9" t="s">
         <v>152</v>
       </c>
@@ -5830,14 +5882,17 @@
       <c r="F9" t="b">
         <v>1</v>
       </c>
-      <c r="M9" t="b">
-        <v>1</v>
-      </c>
-      <c r="P9" t="s">
+      <c r="H9" t="s">
+        <v>152</v>
+      </c>
+      <c r="N9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -5856,8 +5911,11 @@
       <c r="F10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -5876,8 +5934,11 @@
       <c r="F11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19">
       <c r="A12" t="s">
         <v>156</v>
       </c>
@@ -5896,11 +5957,14 @@
       <c r="F12" t="b">
         <v>0</v>
       </c>
-      <c r="M12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H12" t="s">
+        <v>171</v>
+      </c>
+      <c r="N12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
       <c r="A13" t="s">
         <v>157</v>
       </c>
@@ -5919,8 +5983,11 @@
       <c r="F13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -5936,11 +6003,14 @@
       <c r="F14" t="b">
         <v>0</v>
       </c>
-      <c r="M14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H14" s="4">
+        <v>41852</v>
+      </c>
+      <c r="N14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -5956,8 +6026,11 @@
       <c r="F15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H15" s="4">
+        <v>42095</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -5973,8 +6046,11 @@
       <c r="F16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -5990,11 +6066,14 @@
       <c r="F17" t="b">
         <v>1</v>
       </c>
-      <c r="M17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>6</v>
+      </c>
+      <c r="N17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -6010,11 +6089,14 @@
       <c r="F18" t="b">
         <v>0</v>
       </c>
-      <c r="M18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>10.234</v>
+      </c>
+      <c r="N18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -6030,8 +6112,11 @@
       <c r="F19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>15.666</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -6047,11 +6132,14 @@
       <c r="F20" t="b">
         <v>0</v>
       </c>
-      <c r="M20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>173</v>
+      </c>
+      <c r="N20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -6067,8 +6155,11 @@
       <c r="F21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -6087,11 +6178,14 @@
       <c r="G22" t="s">
         <v>81</v>
       </c>
-      <c r="M22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>8</v>
+      </c>
+      <c r="N22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -6110,8 +6204,11 @@
       <c r="G23" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -6127,8 +6224,11 @@
       <c r="F24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -6144,11 +6244,14 @@
       <c r="F25" t="b">
         <v>1</v>
       </c>
-      <c r="M25" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>174</v>
+      </c>
+      <c r="N25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -6164,11 +6267,14 @@
       <c r="F26" t="b">
         <v>0</v>
       </c>
-      <c r="M26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H26" t="s">
+        <v>175</v>
+      </c>
+      <c r="N26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -6184,8 +6290,11 @@
       <c r="F27" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H27" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -6201,11 +6310,14 @@
       <c r="F28" t="b">
         <v>0</v>
       </c>
-      <c r="M28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <v>3</v>
+      </c>
+      <c r="N28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -6221,8 +6333,11 @@
       <c r="F29" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -6238,11 +6353,14 @@
       <c r="F30" t="b">
         <v>0</v>
       </c>
-      <c r="I30">
+      <c r="H30">
+        <v>6</v>
+      </c>
+      <c r="J30">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -6259,10 +6377,13 @@
         <v>1</v>
       </c>
       <c r="H31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -6278,8 +6399,11 @@
       <c r="F32" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>12342151234</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -6295,8 +6419,11 @@
       <c r="F33" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H33">
+        <v>12342151234</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -6313,16 +6440,19 @@
         <v>0</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I34">
+        <v>0</v>
+      </c>
+      <c r="J34">
         <v>10</v>
       </c>
-      <c r="M34" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -6339,16 +6469,19 @@
         <v>1</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
         <v>10</v>
       </c>
-      <c r="M35" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -6367,11 +6500,14 @@
       <c r="F36" t="b">
         <v>0</v>
       </c>
-      <c r="M36" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H36" t="s">
+        <v>171</v>
+      </c>
+      <c r="N36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -6390,8 +6526,11 @@
       <c r="F37" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -6407,11 +6546,14 @@
       <c r="F38" t="b">
         <v>0</v>
       </c>
-      <c r="M38" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H38" t="s">
+        <v>38</v>
+      </c>
+      <c r="N38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -6427,8 +6569,11 @@
       <c r="F39" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -6444,8 +6589,11 @@
       <c r="F40" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -6461,8 +6609,11 @@
       <c r="F41" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -6481,11 +6632,14 @@
       <c r="F42" t="b">
         <v>0</v>
       </c>
-      <c r="M42" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>2</v>
+      </c>
+      <c r="N42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -6504,8 +6658,11 @@
       <c r="F43" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
       <c r="A44" t="s">
         <v>95</v>
       </c>
@@ -6521,11 +6678,14 @@
       <c r="F44" t="b">
         <v>0</v>
       </c>
-      <c r="N44" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
+        <v>38</v>
+      </c>
+      <c r="O44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
       <c r="A45" t="s">
         <v>96</v>
       </c>
@@ -6541,11 +6701,14 @@
       <c r="F45" t="b">
         <v>1</v>
       </c>
-      <c r="N45" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H45" t="s">
+        <v>177</v>
+      </c>
+      <c r="O45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
       <c r="A46" t="s">
         <v>98</v>
       </c>
@@ -6561,11 +6724,11 @@
       <c r="F46" t="b">
         <v>0</v>
       </c>
-      <c r="O46" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
       <c r="A47" t="s">
         <v>100</v>
       </c>
@@ -6581,11 +6744,11 @@
       <c r="F47" t="b">
         <v>0</v>
       </c>
-      <c r="O47" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
       <c r="A48" t="s">
         <v>136</v>
       </c>
@@ -6604,11 +6767,11 @@
       <c r="F48" t="b">
         <v>1</v>
       </c>
-      <c r="O48" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19">
       <c r="A49" t="s">
         <v>143</v>
       </c>
@@ -6627,14 +6790,14 @@
       <c r="F49" t="b">
         <v>1</v>
       </c>
-      <c r="L49" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q49" t="s">
+      <c r="M49" t="b">
+        <v>1</v>
+      </c>
+      <c r="R49" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19">
       <c r="A50" t="s">
         <v>141</v>
       </c>
@@ -6650,14 +6813,14 @@
       <c r="F50" t="b">
         <v>1</v>
       </c>
-      <c r="L50" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q50" t="s">
+      <c r="M50" t="b">
+        <v>1</v>
+      </c>
+      <c r="R50" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19">
       <c r="A51" s="3" t="s">
         <v>147</v>
       </c>
@@ -6678,14 +6841,15 @@
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
-      <c r="L51" s="3"/>
+      <c r="K51" s="3"/>
       <c r="M51" s="3"/>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R51" s="3"/>
+    </row>
+    <row r="52" spans="1:19">
       <c r="A52" s="3" t="s">
         <v>148</v>
       </c>
@@ -6706,17 +6870,18 @@
       <c r="H52" s="3"/>
       <c r="I52" s="3"/>
       <c r="J52" s="3"/>
-      <c r="K52" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="L52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3" t="b">
+        <v>1</v>
+      </c>
       <c r="M52" s="3"/>
-      <c r="O52" s="3"/>
+      <c r="N52" s="3"/>
       <c r="P52" s="3"/>
       <c r="Q52" s="3"/>
       <c r="R52" s="3"/>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S52" s="3"/>
+    </row>
+    <row r="53" spans="1:19">
       <c r="A53" t="s">
         <v>60</v>
       </c>
@@ -6733,7 +6898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19">
       <c r="A54" t="s">
         <v>159</v>
       </c>
@@ -6750,7 +6915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19">
       <c r="A55" t="s">
         <v>162</v>
       </c>
@@ -6766,10 +6931,10 @@
       <c r="F55" t="b">
         <v>1</v>
       </c>
-      <c r="N55" s="3" t="s">
+      <c r="O55" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="R55" t="s">
+      <c r="S55" t="s">
         <v>164</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Validate attribute metadata with defaultValue.
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
+++ b/molgenis-app/src/test/resources/emx_all_datatypes.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="176">
   <si>
     <t>text</t>
   </si>
@@ -530,12 +530,6 @@
   </si>
   <si>
     <t>defaultValue</t>
-  </si>
-  <si>
-    <t>typeTestRef</t>
-  </si>
-  <si>
-    <t>typeTestRefLabel</t>
   </si>
   <si>
     <t>ref1,ref2</t>
@@ -5632,8 +5626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5724,9 +5718,6 @@
       <c r="F2" t="b">
         <v>0</v>
       </c>
-      <c r="H2" t="s">
-        <v>169</v>
-      </c>
       <c r="K2" t="b">
         <v>1</v>
       </c>
@@ -5747,9 +5738,6 @@
       <c r="F3" t="b">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
-        <v>170</v>
-      </c>
       <c r="K3" t="b">
         <v>1</v>
       </c>
@@ -5958,7 +5946,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="N12" t="b">
         <v>1</v>
@@ -5984,7 +5972,7 @@
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:19">
@@ -6133,7 +6121,7 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="N20" t="b">
         <v>1</v>
@@ -6245,7 +6233,7 @@
         <v>1</v>
       </c>
       <c r="H25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="N25" t="b">
         <v>1</v>
@@ -6268,7 +6256,7 @@
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="N26" t="b">
         <v>1</v>
@@ -6291,7 +6279,7 @@
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -6500,9 +6488,6 @@
       <c r="F36" t="b">
         <v>0</v>
       </c>
-      <c r="H36" t="s">
-        <v>171</v>
-      </c>
       <c r="N36" t="b">
         <v>1</v>
       </c>
@@ -6526,9 +6511,6 @@
       <c r="F37" t="b">
         <v>1</v>
       </c>
-      <c r="H37" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="38" spans="1:16">
       <c r="A38" t="s">
@@ -6632,9 +6614,6 @@
       <c r="F42" t="b">
         <v>0</v>
       </c>
-      <c r="H42" t="s">
-        <v>2</v>
-      </c>
       <c r="N42" t="b">
         <v>1</v>
       </c>
@@ -6658,9 +6637,6 @@
       <c r="F43" t="b">
         <v>1</v>
       </c>
-      <c r="H43" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="44" spans="1:16">
       <c r="A44" t="s">
@@ -6702,7 +6678,7 @@
         <v>1</v>
       </c>
       <c r="H45" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="O45" t="b">
         <v>0</v>

</xml_diff>